<commit_message>
a ready version for submit
</commit_message>
<xml_diff>
--- a/data/performance.xlsx
+++ b/data/performance.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="413">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1554,59 +1554,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[3]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[13]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>[24]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[57]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[5]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[70]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[72]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[35]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[46]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[54]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[69]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[11]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[33]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>[44]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[44]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[51]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[62]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[48]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[40]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[59]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[8]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[28]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[38]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[34]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[21]</t>
+    <t>[27]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1614,39 +1626,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[24]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[27]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[61]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[11]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[57]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[9]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[58]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[60]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[30]</t>
+    <t>[71]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[14]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[65]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[12]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[68]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[50]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[50]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2145,10 +2149,43 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2169,43 +2206,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2344,7 +2348,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF573468-0D1C-47DC-9171-27D883B53F25}" type="CELLRANGE">
+                    <a:fld id="{A289A1D4-1F0D-4930-AC24-20C2ECBE4EBD}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2377,7 +2381,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F540C997-FFAF-4C58-A50F-3EBC6A8AB574}" type="CELLRANGE">
+                    <a:fld id="{F409329B-7106-4FFF-952B-8C700AEAF7B5}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2410,7 +2414,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC6CE33F-8DE3-404D-82A4-BD5D8EA5968D}" type="CELLRANGE">
+                    <a:fld id="{24E576E5-DBB7-4F95-AB35-665478810E64}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2443,7 +2447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EB9195D-01A6-4E53-81D5-6FF6D8701827}" type="CELLRANGE">
+                    <a:fld id="{A240411A-6F48-4C48-A21A-16FEDB598DA2}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2476,7 +2480,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6EDCE76D-B059-454C-B664-531E8970E5C2}" type="CELLRANGE">
+                    <a:fld id="{C6F9CD30-3C72-48B0-8F71-2BF083E3A57E}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2509,7 +2513,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DC55065-1478-4939-90E3-E453F29057CE}" type="CELLRANGE">
+                    <a:fld id="{92E5AD14-F9EA-4F35-AFB4-4FC8186952E7}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2542,7 +2546,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EF1D7B9-F9FA-4AB1-8DD0-DA5C1F7377BF}" type="CELLRANGE">
+                    <a:fld id="{B158559C-2F5C-4E92-BD0A-FC1BEACACC5E}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2599,7 +2603,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47651668-B2BE-494E-90F2-015D568DCD3E}" type="CELLRANGE">
+                    <a:fld id="{0B1560CA-4B14-434E-A2B9-9B6E2D96D2B9}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2632,7 +2636,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D917AA5-F75C-4230-9A24-BDBB76937D1B}" type="CELLRANGE">
+                    <a:fld id="{FB07B301-A427-4B22-A96C-9F5F5B16277B}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2665,7 +2669,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{501C359D-C248-4A89-B7DA-FD9BA6F36FDF}" type="CELLRANGE">
+                    <a:fld id="{37CAC468-7B65-4E81-9832-ECAEAECB9D04}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2722,7 +2726,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7A43E67-E4B6-407E-9EF2-BB712FC65CC9}" type="CELLRANGE">
+                    <a:fld id="{DE13296D-F842-4675-BEB1-501B41567BF9}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2755,7 +2759,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B27DCB3-63DE-4AB2-92E4-C4DAD95C92A8}" type="CELLRANGE">
+                    <a:fld id="{A117FF8F-8C3E-41CF-89DE-61267D57D6D5}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2788,7 +2792,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3078007E-C622-4707-88A9-7DC21F6790D6}" type="CELLRANGE">
+                    <a:fld id="{2C6386B6-D4FF-430D-95D4-0CC32B7CF53D}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2821,7 +2825,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E7B4136-E935-4F15-A9F3-82570434B7A2}" type="CELLRANGE">
+                    <a:fld id="{B2E14483-63C8-4E08-8BC9-0424D6DE3459}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2878,7 +2882,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{360FB0BD-20E4-4E8B-A433-171A79A2E927}" type="CELLRANGE">
+                    <a:fld id="{E72B088C-D492-4286-BF85-5F6B4C2CF1FC}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2935,7 +2939,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{404D7C93-8DBE-4B3B-8BE4-ADC683BABFB1}" type="CELLRANGE">
+                    <a:fld id="{6033F82B-B91E-4D1B-B248-73130C594AA9}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2992,7 +2996,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8DC7A03-2432-46F2-9F15-ECEBF08D2E6B}" type="CELLRANGE">
+                    <a:fld id="{6F2B7FB1-1BDC-4DB1-BE07-C74CF3BA3D54}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3049,7 +3053,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72CCD009-E76F-45EB-AC76-A3901B945555}" type="CELLRANGE">
+                    <a:fld id="{94D53E77-A67E-46FC-9173-2BCEB88AD499}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3106,7 +3110,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DAA8DF5-BE1A-41AD-A3CD-FC8C7F87A331}" type="CELLRANGE">
+                    <a:fld id="{01DF72DF-717C-4CB4-B837-3C8492C89212}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4685,7 +4689,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{579F3E79-FDF3-4CC2-81D0-AFE43FAA5617}" type="CELLRANGE">
+                    <a:fld id="{0FC4C73D-09E9-4228-B353-84E027A1ADC9}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5592,82 +5596,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -6610,82 +6614,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -7667,82 +7671,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -7937,7 +7941,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6B3A662-D3BD-47C2-9967-6C0BF8765420}" type="CELLRANGE">
+                    <a:fld id="{87D48914-4608-41A5-BA81-D3DA37ED3B25}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8762,82 +8766,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -9099,7 +9103,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F0BE6D6-0F28-4C27-9B6F-873590CCA0E4}" type="CELLRANGE">
+                    <a:fld id="{748F7ED1-63D1-4579-8477-3CB65B6CFA78}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9808,82 +9812,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -10232,7 +10236,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{639CFF9E-F0BB-4608-A5BB-6E7BE59FF6FC}" type="CELLRANGE">
+                    <a:fld id="{713327D7-580E-4A22-A619-F2351CE25CD9}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11026,82 +11030,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -11640,7 +11644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8023BAD3-3B13-47B7-9671-00F58B20D64A}" type="CELLRANGE">
+                    <a:fld id="{4BFE932D-9C6A-4ECA-BF63-A19E8E56F0AD}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12058,82 +12062,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -13124,82 +13128,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -13869,7 +13873,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0004A307-2D3A-4A8C-9F4A-482E60170031}" type="CELLRANGE">
+                    <a:fld id="{5B9330D7-8768-4DDF-9D2A-B6F786AB9AF2}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13904,7 +13908,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE2FD431-9F63-4AAE-8464-B0C752D9EF57}" type="CELLRANGE">
+                    <a:fld id="{B20C2E50-4CE5-4787-89F8-5E54AFB7A262}" type="CELLRANGE">
                       <a:rPr lang="zh-CN" altLang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14211,82 +14215,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="26"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -15292,82 +15296,82 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="31"/>
                   <c:pt idx="0">
-                    <c:v>[34]</c:v>
+                    <c:v>[40]</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>[38]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>[24]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>[14]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>[35]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>[54]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>[32]</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>[21]</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>[11]</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>[30]</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>[48]</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>[27]</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>[13]</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>[13]</c:v>
+                    <c:v>[16]</c:v>
                   </c:pt>
                   <c:pt idx="9">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>[50]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>[57]</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>[72]</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>[46]</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>[11]</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>[33]</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>[27]</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>[71]</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>[65]</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>[68]</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>[5]</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>[44]</c:v>
                   </c:pt>
-                  <c:pt idx="10">
-                    <c:v>[44]</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>[51]</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>[62]</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>[40]</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>[8]</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>[28]</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>[24]</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>[61]</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>[57]</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>[58]</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>[3]</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>[38]</c:v>
-                  </c:pt>
                   <c:pt idx="22">
-                    <c:v>[60]</c:v>
+                    <c:v>[70]</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>[62]</c:v>
+                    <c:v>[72]</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>[59]</c:v>
+                    <c:v>[69]</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>[9]</c:v>
+                    <c:v>[12]</c:v>
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>Nvidia TX1(batch-1)</c:v>
@@ -25320,8 +25324,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="62"/>
-      <c r="B1" s="44"/>
+      <c r="A1" s="46"/>
+      <c r="B1" s="47"/>
       <c r="C1" s="15" t="s">
         <v>304</v>
       </c>
@@ -25337,33 +25341,33 @@
       <c r="G1" s="37" t="s">
         <v>370</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="53" t="s">
         <v>297</v>
       </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="39" t="s">
         <v>372</v>
       </c>
-      <c r="L1" s="56" t="s">
+      <c r="L1" s="51" t="s">
         <v>293</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="N1" s="47" t="s">
         <v>306</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="O1" s="47" t="s">
         <v>317</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="55" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="62"/>
-      <c r="B2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="16" t="s">
         <v>305</v>
       </c>
@@ -25391,11 +25395,11 @@
       <c r="K2" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="53"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -25590,10 +25594,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="B7" s="44"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="5" t="s">
         <v>324</v>
       </c>
@@ -25621,25 +25625,25 @@
       <c r="K7" s="30">
         <v>20</v>
       </c>
-      <c r="L7" s="44" t="s">
+      <c r="L7" s="47" t="s">
         <v>289</v>
       </c>
-      <c r="M7" s="44" t="s">
+      <c r="M7" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="N7" s="44" t="s">
+      <c r="N7" s="47" t="s">
         <v>307</v>
       </c>
-      <c r="O7" s="44">
+      <c r="O7" s="47">
         <v>17</v>
       </c>
-      <c r="P7" s="46" t="s">
+      <c r="P7" s="57" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="9" t="s">
         <v>325</v>
       </c>
@@ -25667,11 +25671,11 @@
       <c r="K8" s="30">
         <v>20</v>
       </c>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="47"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="58"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -26244,72 +26248,72 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="47" t="s">
         <v>354</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44" t="s">
+      <c r="B21" s="47"/>
+      <c r="C21" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="D21" s="63">
+      <c r="D21" s="49">
         <v>1280.3</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E21" s="59">
         <v>160</v>
       </c>
-      <c r="F21" s="50">
+      <c r="F21" s="61">
         <v>8</v>
       </c>
-      <c r="G21" s="54">
+      <c r="G21" s="63">
         <v>150</v>
       </c>
-      <c r="H21" s="44" t="s">
+      <c r="H21" s="47" t="s">
         <v>336</v>
       </c>
-      <c r="I21" s="44" t="s">
+      <c r="I21" s="47" t="s">
         <v>337</v>
       </c>
-      <c r="J21" s="52" t="s">
+      <c r="J21" s="55" t="s">
         <v>338</v>
       </c>
-      <c r="K21" s="44">
+      <c r="K21" s="47">
         <v>28</v>
       </c>
       <c r="L21" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="M21" s="44" t="s">
+      <c r="M21" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="N21" s="44" t="s">
+      <c r="N21" s="47" t="s">
         <v>311</v>
       </c>
-      <c r="O21" s="44">
+      <c r="O21" s="47">
         <v>16</v>
       </c>
-      <c r="P21" s="46" t="s">
+      <c r="P21" s="57" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="45"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="45"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="48"/>
       <c r="L22" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="47"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="58"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -26504,12 +26508,12 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="44" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C28" s="61"/>
+      <c r="C28" s="45"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C32" s="17"/>
@@ -26528,26 +26532,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
     <mergeCell ref="M21:M22"/>
     <mergeCell ref="N21:N22"/>
     <mergeCell ref="O21:O22"/>
@@ -26559,6 +26543,26 @@
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26571,8 +26575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -26581,12 +26585,16 @@
     <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.75" customWidth="1"/>
-    <col min="7" max="7" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" customWidth="1"/>
-    <col min="15" max="15" width="16.5" customWidth="1"/>
-    <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="20.25" customWidth="1"/>
+    <col min="6" max="7" width="6.75" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="10" max="10" width="6.625" customWidth="1"/>
+    <col min="11" max="11" width="7.375" customWidth="1"/>
+    <col min="12" max="12" width="7.25" customWidth="1"/>
+    <col min="13" max="13" width="6.875" customWidth="1"/>
+    <col min="14" max="14" width="7.5" customWidth="1"/>
+    <col min="15" max="15" width="9.375" customWidth="1"/>
+    <col min="16" max="16" width="9.875" customWidth="1"/>
+    <col min="17" max="17" width="10.625" customWidth="1"/>
     <col min="18" max="18" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -26676,7 +26684,7 @@
       <c r="O2" s="27"/>
       <c r="P2" s="27"/>
       <c r="Q2" s="29" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="R2" s="29" t="s">
         <v>318</v>
@@ -26718,7 +26726,7 @@
       <c r="O3" s="27"/>
       <c r="P3" s="27"/>
       <c r="Q3" s="29" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="R3" s="29" t="s">
         <v>343</v>
@@ -26760,7 +26768,7 @@
       <c r="O4" s="27"/>
       <c r="P4" s="27"/>
       <c r="Q4" s="29" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="R4" s="29" t="s">
         <v>339</v>
@@ -26802,7 +26810,7 @@
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
       <c r="Q5" s="29" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="R5" s="29" t="s">
         <v>340</v>
@@ -26845,7 +26853,7 @@
       <c r="O6" s="27"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="29" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="R6" s="29" t="s">
         <v>345</v>
@@ -26887,7 +26895,7 @@
       <c r="O7" s="27"/>
       <c r="P7" s="27"/>
       <c r="Q7" s="29" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="R7" s="29" t="s">
         <v>346</v>
@@ -26929,7 +26937,7 @@
       <c r="O8" s="27"/>
       <c r="P8" s="27"/>
       <c r="Q8" s="29" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="R8" s="29" t="s">
         <v>347</v>
@@ -26971,7 +26979,7 @@
       <c r="O9" s="27"/>
       <c r="P9" s="27"/>
       <c r="Q9" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="R9" s="29" t="s">
         <v>348</v>
@@ -27013,7 +27021,7 @@
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
       <c r="Q10" s="29" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="R10" s="29" t="s">
         <v>348</v>
@@ -27055,7 +27063,7 @@
       <c r="O11" s="27"/>
       <c r="P11" s="27"/>
       <c r="Q11" s="29" t="s">
-        <v>390</v>
+        <v>411</v>
       </c>
       <c r="R11" s="29" t="s">
         <v>382</v>
@@ -27097,7 +27105,7 @@
       <c r="O12" s="27"/>
       <c r="P12" s="27"/>
       <c r="Q12" s="29" t="s">
-        <v>391</v>
+        <v>412</v>
       </c>
       <c r="R12" s="29" t="s">
         <v>382</v>
@@ -27139,7 +27147,7 @@
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
       <c r="Q13" s="29" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="R13" s="29" t="s">
         <v>320</v>
@@ -27181,7 +27189,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
       <c r="Q14" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="R14" s="29" t="s">
         <v>385</v>
@@ -27223,7 +27231,7 @@
       <c r="O15" s="27"/>
       <c r="P15" s="27"/>
       <c r="Q15" s="29" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="R15" s="29" t="s">
         <v>350</v>
@@ -27265,7 +27273,7 @@
       <c r="O16" s="27"/>
       <c r="P16" s="27"/>
       <c r="Q16" s="29" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="R16" s="29" t="s">
         <v>351</v>
@@ -27307,7 +27315,7 @@
       <c r="O17" s="27"/>
       <c r="P17" s="27"/>
       <c r="Q17" s="29" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="R17" s="29" t="s">
         <v>352</v>
@@ -27349,7 +27357,7 @@
       <c r="O18" s="27"/>
       <c r="P18" s="27"/>
       <c r="Q18" s="29" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="R18" s="29" t="s">
         <v>353</v>
@@ -27391,7 +27399,7 @@
       <c r="O19" s="27"/>
       <c r="P19" s="27"/>
       <c r="Q19" s="29" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="R19" s="29" t="s">
         <v>354</v>
@@ -27433,7 +27441,7 @@
       <c r="O20" s="27"/>
       <c r="P20" s="27"/>
       <c r="Q20" s="29" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="R20" s="29" t="s">
         <v>355</v>
@@ -27475,7 +27483,7 @@
       <c r="O21" s="27"/>
       <c r="P21" s="27"/>
       <c r="Q21" s="29" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="R21" s="29" t="s">
         <v>356</v>
@@ -27517,7 +27525,7 @@
       <c r="O22" s="27"/>
       <c r="P22" s="27"/>
       <c r="Q22" s="29" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="R22" s="29" t="s">
         <v>319</v>
@@ -27559,7 +27567,7 @@
       <c r="O23" s="27"/>
       <c r="P23" s="27"/>
       <c r="Q23" s="29" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="R23" s="29" t="s">
         <v>357</v>
@@ -27601,7 +27609,7 @@
       <c r="O24" s="27"/>
       <c r="P24" s="27"/>
       <c r="Q24" s="29" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="R24" s="29" t="s">
         <v>386</v>
@@ -27643,7 +27651,7 @@
       <c r="O25" s="27"/>
       <c r="P25" s="27"/>
       <c r="Q25" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="R25" s="29" t="s">
         <v>385</v>
@@ -27681,7 +27689,7 @@
       <c r="O26" s="27"/>
       <c r="P26" s="27"/>
       <c r="Q26" s="29" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="R26" s="29" t="s">
         <v>359</v>
@@ -27711,7 +27719,7 @@
       <c r="O27" s="27"/>
       <c r="P27" s="27"/>
       <c r="Q27" s="29" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="R27" s="29" t="s">
         <v>360</v>

</xml_diff>